<commit_message>
Built up simulation for presentation.
Presentation & script will be uploaded w/ next commit
</commit_message>
<xml_diff>
--- a/modelling/PR48_data1 (1).xlsx
+++ b/modelling/PR48_data1 (1).xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben\Desktop\gitrepos\physics-project\modelling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56EDA2D2-6AF5-4398-961D-FFDF08A80095}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A6374F1-8B0C-4731-BF48-3EFA2E89B95D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{EA0F97A9-31C8-4344-91CC-B13EDB70A7C8}"/>
+    <workbookView xWindow="-28920" yWindow="-1935" windowWidth="29040" windowHeight="15840" xr2:uid="{EA0F97A9-31C8-4344-91CC-B13EDB70A7C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>16 reflective strips.</t>
   </si>
@@ -62,9 +62,6 @@
     <t xml:space="preserve">Coil current </t>
   </si>
   <si>
-    <t>A (+-0.0005)</t>
-  </si>
-  <si>
     <t>30cm Aluminium disc.</t>
   </si>
   <si>
@@ -150,6 +147,12 @@
   </si>
   <si>
     <t>RC4</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>(+-0.0005)</t>
   </si>
 </sst>
 </file>
@@ -503,8 +506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51327C71-5F81-44A9-838C-25FE6C5F69BE}">
   <dimension ref="A1:AE26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C128" sqref="A103:C128"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="AC21" sqref="AC21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,13 +518,16 @@
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
       </c>
       <c r="G1" t="s">
         <v>0</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.25">
@@ -546,91 +552,91 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3" t="s">
+        <v>19</v>
+      </c>
+      <c r="M3" t="s">
+        <v>20</v>
+      </c>
+      <c r="N3" t="s">
         <v>22</v>
       </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K3" t="s">
-        <v>19</v>
-      </c>
-      <c r="L3" t="s">
-        <v>20</v>
-      </c>
-      <c r="M3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>23</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>24</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>25</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>26</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>27</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
         <v>28</v>
       </c>
-      <c r="T3" t="s">
+      <c r="U3" t="s">
         <v>29</v>
       </c>
-      <c r="U3" t="s">
+      <c r="V3" t="s">
         <v>30</v>
       </c>
-      <c r="V3" t="s">
+      <c r="W3" t="s">
         <v>31</v>
       </c>
-      <c r="W3" t="s">
+      <c r="X3" t="s">
         <v>32</v>
       </c>
-      <c r="X3" t="s">
+      <c r="Y3" t="s">
         <v>33</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="Z3" t="s">
         <v>34</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="AA3" t="s">
         <v>35</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AB3" t="s">
         <v>36</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="AC3" t="s">
         <v>37</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AD3" t="s">
         <v>38</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>9</v>
       </c>
       <c r="AE3" t="s">
         <v>6</v>

</xml_diff>